<commit_message>
Add feature tests for Affiliate endpoints and setup TestCase
- Created AffiliateEndpointsTest to test policies, index, show, create, update, delete, restore, force delete, and export functionalities for Affiliate model.
- Created AffiliateLinkEndpointsTest for testing similar functionalities for AffiliateLink model.
- Created AffiliatePayoutEndpointsTest for testing functionalities related to AffiliatePayout model.
- Created AffiliateProgramEndpointsTest for testing functionalities related to AffiliateProgram model.
- Added a base TestCase class for setting up tests with necessary configurations.
</commit_message>
<xml_diff>
--- a/docs/DevelopChecklist.xlsx
+++ b/docs/DevelopChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\innoboxrr\packages\affiliate-saas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585480AD-1A2C-4C22-A0F0-D93B43DD1DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855CC96A-4FF6-47B9-A831-A51ACE945714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4B8113D-0672-4603-BE1D-648575D65001}"/>
   </bookViews>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
   <si>
     <t>Backend</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>AffilaitePayout</t>
+  </si>
+  <si>
+    <t>Affiliate</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -905,9 +908,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -915,6 +915,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -926,25 +947,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1327,13 +1333,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DL15"/>
+  <dimension ref="B1:DL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1363,279 +1369,279 @@
     <col min="115" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="38"/>
-      <c r="C1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="42"/>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AI1" s="42"/>
-      <c r="AJ1" s="42"/>
-      <c r="AK1" s="42"/>
-      <c r="AL1" s="42"/>
-      <c r="AM1" s="42"/>
-      <c r="AN1" s="42"/>
-      <c r="AO1" s="42"/>
-      <c r="AP1" s="42"/>
-      <c r="AQ1" s="42"/>
-      <c r="AR1" s="42"/>
-      <c r="AS1" s="42"/>
-      <c r="AT1" s="42"/>
-      <c r="AU1" s="42"/>
-      <c r="AV1" s="42"/>
-      <c r="AW1" s="42"/>
-      <c r="AX1" s="42"/>
-      <c r="AY1" s="42"/>
-      <c r="AZ1" s="42"/>
-      <c r="BA1" s="42"/>
-      <c r="BB1" s="42"/>
-      <c r="BC1" s="42"/>
-      <c r="BD1" s="42"/>
-      <c r="BE1" s="42"/>
-      <c r="BF1" s="42"/>
-      <c r="BG1" s="42"/>
-      <c r="BH1" s="42"/>
-      <c r="BI1" s="42"/>
-      <c r="BJ1" s="42"/>
-      <c r="BK1" s="42"/>
-      <c r="BL1" s="42"/>
-      <c r="BM1" s="42"/>
-      <c r="BN1" s="42"/>
-      <c r="BO1" s="42"/>
-      <c r="BP1" s="42"/>
-      <c r="BQ1" s="42"/>
-      <c r="BR1" s="42"/>
-      <c r="BS1" s="42"/>
-      <c r="BT1" s="42"/>
-      <c r="BU1" s="42"/>
-      <c r="BV1" s="42"/>
-      <c r="BW1" s="42"/>
-      <c r="BX1" s="42"/>
-      <c r="BY1" s="42"/>
-      <c r="BZ1" s="42"/>
-      <c r="CA1" s="42"/>
-      <c r="CB1" s="42"/>
-      <c r="CC1" s="42"/>
-      <c r="CD1" s="42"/>
-      <c r="CE1" s="42"/>
-      <c r="CF1" s="42"/>
-      <c r="CG1" s="42"/>
-      <c r="CH1" s="42"/>
-      <c r="CI1" s="42"/>
-      <c r="CJ1" s="42"/>
-      <c r="CK1" s="42"/>
-      <c r="CL1" s="42"/>
-      <c r="CM1" s="42"/>
-      <c r="CN1" s="42"/>
-      <c r="CO1" s="30" t="s">
+    <row r="1" spans="2:116" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="33"/>
+      <c r="C1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38"/>
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="38"/>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38"/>
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38"/>
+      <c r="BD1" s="38"/>
+      <c r="BE1" s="38"/>
+      <c r="BF1" s="38"/>
+      <c r="BG1" s="38"/>
+      <c r="BH1" s="38"/>
+      <c r="BI1" s="38"/>
+      <c r="BJ1" s="38"/>
+      <c r="BK1" s="38"/>
+      <c r="BL1" s="38"/>
+      <c r="BM1" s="38"/>
+      <c r="BN1" s="38"/>
+      <c r="BO1" s="38"/>
+      <c r="BP1" s="38"/>
+      <c r="BQ1" s="38"/>
+      <c r="BR1" s="38"/>
+      <c r="BS1" s="38"/>
+      <c r="BT1" s="38"/>
+      <c r="BU1" s="38"/>
+      <c r="BV1" s="38"/>
+      <c r="BW1" s="38"/>
+      <c r="BX1" s="38"/>
+      <c r="BY1" s="38"/>
+      <c r="BZ1" s="38"/>
+      <c r="CA1" s="38"/>
+      <c r="CB1" s="38"/>
+      <c r="CC1" s="38"/>
+      <c r="CD1" s="38"/>
+      <c r="CE1" s="38"/>
+      <c r="CF1" s="38"/>
+      <c r="CG1" s="38"/>
+      <c r="CH1" s="38"/>
+      <c r="CI1" s="38"/>
+      <c r="CJ1" s="38"/>
+      <c r="CK1" s="38"/>
+      <c r="CL1" s="38"/>
+      <c r="CM1" s="38"/>
+      <c r="CN1" s="38"/>
+      <c r="CO1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="CP1" s="30"/>
-      <c r="CQ1" s="30"/>
-      <c r="CR1" s="30"/>
-      <c r="CS1" s="30"/>
-      <c r="CT1" s="30"/>
-      <c r="CU1" s="30"/>
-      <c r="CV1" s="30"/>
-      <c r="CW1" s="30"/>
-      <c r="CX1" s="30"/>
-      <c r="CY1" s="30"/>
-      <c r="CZ1" s="30"/>
-      <c r="DA1" s="30"/>
-      <c r="DB1" s="30"/>
-      <c r="DC1" s="30"/>
-      <c r="DD1" s="30"/>
-      <c r="DE1" s="30"/>
-      <c r="DF1" s="30"/>
-      <c r="DG1" s="30"/>
-      <c r="DH1" s="30"/>
-      <c r="DI1" s="30"/>
+      <c r="CP1" s="39"/>
+      <c r="CQ1" s="39"/>
+      <c r="CR1" s="39"/>
+      <c r="CS1" s="39"/>
+      <c r="CT1" s="39"/>
+      <c r="CU1" s="39"/>
+      <c r="CV1" s="39"/>
+      <c r="CW1" s="39"/>
+      <c r="CX1" s="39"/>
+      <c r="CY1" s="39"/>
+      <c r="CZ1" s="39"/>
+      <c r="DA1" s="39"/>
+      <c r="DB1" s="39"/>
+      <c r="DC1" s="39"/>
+      <c r="DD1" s="39"/>
+      <c r="DE1" s="39"/>
+      <c r="DF1" s="39"/>
+      <c r="DG1" s="39"/>
+      <c r="DH1" s="39"/>
+      <c r="DI1" s="39"/>
       <c r="DK1" s="7" t="s">
         <v>75</v>
       </c>
       <c r="DL1" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:116" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39"/>
-      <c r="C2" s="31" t="s">
+    <row r="2" spans="2:116" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34"/>
+      <c r="C2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="31" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="31" t="s">
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="33"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="32"/>
       <c r="AD2" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="AE2" s="31" t="s">
+      <c r="AE2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="31" t="s">
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="31" t="s">
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-      <c r="AY2" s="32"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="31" t="s">
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
+      <c r="AW2" s="31"/>
+      <c r="AX2" s="31"/>
+      <c r="AY2" s="31"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="BB2" s="32"/>
-      <c r="BC2" s="32"/>
-      <c r="BD2" s="32"/>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="33"/>
+      <c r="BB2" s="31"/>
+      <c r="BC2" s="31"/>
+      <c r="BD2" s="31"/>
+      <c r="BE2" s="31"/>
+      <c r="BF2" s="32"/>
       <c r="BG2" s="18" t="s">
         <v>83</v>
       </c>
       <c r="BH2" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="BI2" s="31" t="s">
+      <c r="BI2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="BJ2" s="32"/>
-      <c r="BK2" s="32"/>
-      <c r="BL2" s="32"/>
-      <c r="BM2" s="32"/>
-      <c r="BN2" s="32"/>
-      <c r="BO2" s="32"/>
-      <c r="BP2" s="32"/>
-      <c r="BQ2" s="33"/>
+      <c r="BJ2" s="31"/>
+      <c r="BK2" s="31"/>
+      <c r="BL2" s="31"/>
+      <c r="BM2" s="31"/>
+      <c r="BN2" s="31"/>
+      <c r="BO2" s="31"/>
+      <c r="BP2" s="31"/>
+      <c r="BQ2" s="32"/>
       <c r="BR2" s="21"/>
-      <c r="BS2" s="31" t="s">
+      <c r="BS2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="BT2" s="32"/>
-      <c r="BU2" s="32"/>
-      <c r="BV2" s="32"/>
-      <c r="BW2" s="32"/>
-      <c r="BX2" s="32"/>
-      <c r="BY2" s="32"/>
-      <c r="BZ2" s="32"/>
-      <c r="CA2" s="32"/>
-      <c r="CB2" s="32"/>
-      <c r="CC2" s="32"/>
-      <c r="CD2" s="33"/>
-      <c r="CE2" s="31" t="s">
+      <c r="BT2" s="31"/>
+      <c r="BU2" s="31"/>
+      <c r="BV2" s="31"/>
+      <c r="BW2" s="31"/>
+      <c r="BX2" s="31"/>
+      <c r="BY2" s="31"/>
+      <c r="BZ2" s="31"/>
+      <c r="CA2" s="31"/>
+      <c r="CB2" s="31"/>
+      <c r="CC2" s="31"/>
+      <c r="CD2" s="32"/>
+      <c r="CE2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="CF2" s="32"/>
-      <c r="CG2" s="32"/>
-      <c r="CH2" s="32"/>
-      <c r="CI2" s="32"/>
-      <c r="CJ2" s="32"/>
-      <c r="CK2" s="32"/>
-      <c r="CL2" s="32"/>
-      <c r="CM2" s="32"/>
-      <c r="CN2" s="37"/>
-      <c r="CO2" s="31" t="s">
+      <c r="CF2" s="31"/>
+      <c r="CG2" s="31"/>
+      <c r="CH2" s="31"/>
+      <c r="CI2" s="31"/>
+      <c r="CJ2" s="31"/>
+      <c r="CK2" s="31"/>
+      <c r="CL2" s="31"/>
+      <c r="CM2" s="31"/>
+      <c r="CN2" s="36"/>
+      <c r="CO2" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="CP2" s="32"/>
-      <c r="CQ2" s="33"/>
-      <c r="CR2" s="34" t="s">
+      <c r="CP2" s="31"/>
+      <c r="CQ2" s="32"/>
+      <c r="CR2" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="CS2" s="35"/>
-      <c r="CT2" s="35"/>
-      <c r="CU2" s="35"/>
-      <c r="CV2" s="36"/>
-      <c r="CW2" s="31" t="s">
+      <c r="CS2" s="41"/>
+      <c r="CT2" s="41"/>
+      <c r="CU2" s="41"/>
+      <c r="CV2" s="42"/>
+      <c r="CW2" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="CX2" s="32"/>
-      <c r="CY2" s="32"/>
-      <c r="CZ2" s="32"/>
-      <c r="DA2" s="32"/>
-      <c r="DB2" s="32"/>
-      <c r="DC2" s="33"/>
-      <c r="DD2" s="31" t="s">
+      <c r="CX2" s="31"/>
+      <c r="CY2" s="31"/>
+      <c r="CZ2" s="31"/>
+      <c r="DA2" s="31"/>
+      <c r="DB2" s="31"/>
+      <c r="DC2" s="32"/>
+      <c r="DD2" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="DE2" s="33"/>
-      <c r="DF2" s="31" t="s">
+      <c r="DE2" s="32"/>
+      <c r="DF2" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="DG2" s="32"/>
-      <c r="DH2" s="37"/>
-      <c r="DI2" s="33"/>
+      <c r="DG2" s="31"/>
+      <c r="DH2" s="36"/>
+      <c r="DI2" s="32"/>
       <c r="DK2" s="7" t="s">
         <v>76</v>
       </c>
@@ -1643,8 +1649,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:116" s="4" customFormat="1" ht="95.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
+    <row r="3" spans="2:116" s="4" customFormat="1" ht="95.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="35"/>
       <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
@@ -1985,16 +1991,13 @@
         <v>68</v>
       </c>
       <c r="DL3" s="8">
-        <f>SUM(DJ13,DJ15)*100/(DL2*DL1) * 0.01</f>
+        <f>SUM(DJ14,DJ16)*100/(DL2*DL1) * 0.01</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
+    <row r="4" spans="2:116" x14ac:dyDescent="0.3">
       <c r="B4" s="43" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="9"/>
@@ -2112,16 +2115,13 @@
         <v>111</v>
       </c>
       <c r="DK4" s="3">
-        <f t="shared" ref="DK4:DK10" si="0">DJ4/$DL$2</f>
+        <f t="shared" ref="DK4:DK11" si="0">DJ4/$DL$2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>106</v>
+    <row r="5" spans="2:116" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="9"/>
@@ -2234,18 +2234,11 @@
       <c r="DG5" s="9"/>
       <c r="DH5" s="9"/>
       <c r="DI5" s="29"/>
-      <c r="DJ5" s="1">
-        <f t="shared" ref="DJ5:DJ10" si="1">COUNTIF(C5:DI5,"")</f>
-        <v>111</v>
-      </c>
-      <c r="DK5" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="DK5" s="3"/>
     </row>
-    <row r="6" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:116" x14ac:dyDescent="0.3">
       <c r="B6" s="26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="9"/>
@@ -2359,7 +2352,7 @@
       <c r="DH6" s="9"/>
       <c r="DI6" s="29"/>
       <c r="DJ6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="DJ6:DJ11" si="1">COUNTIF(C6:DI6,"")</f>
         <v>111</v>
       </c>
       <c r="DK6" s="3">
@@ -2367,9 +2360,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:116" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="9"/>
@@ -2491,12 +2484,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
+    <row r="8" spans="2:116" x14ac:dyDescent="0.3">
       <c r="B8" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="9"/>
@@ -2618,9 +2608,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:116" x14ac:dyDescent="0.3">
       <c r="B9" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="9"/>
@@ -2742,9 +2732,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
-        <v>110</v>
+    <row r="10" spans="2:116" x14ac:dyDescent="0.3">
+      <c r="B10" s="44" t="s">
+        <v>109</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="9"/>
@@ -2866,1825 +2856,1955 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="DJ11" s="6"/>
+    <row r="11" spans="2:116" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="16"/>
+      <c r="AD11" s="25"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" s="12"/>
+      <c r="AK11" s="12"/>
+      <c r="AL11" s="12"/>
+      <c r="AM11" s="12"/>
+      <c r="AN11" s="12"/>
+      <c r="AO11" s="12"/>
+      <c r="AP11" s="16"/>
+      <c r="AQ11" s="17"/>
+      <c r="AR11" s="12"/>
+      <c r="AS11" s="12"/>
+      <c r="AT11" s="12"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="12"/>
+      <c r="AX11" s="12"/>
+      <c r="AY11" s="12"/>
+      <c r="AZ11" s="16"/>
+      <c r="BA11" s="17"/>
+      <c r="BB11" s="12"/>
+      <c r="BC11" s="12"/>
+      <c r="BD11" s="12"/>
+      <c r="BE11" s="12"/>
+      <c r="BF11" s="16"/>
+      <c r="BG11" s="20"/>
+      <c r="BH11" s="20"/>
+      <c r="BI11" s="17"/>
+      <c r="BJ11" s="12"/>
+      <c r="BK11" s="12"/>
+      <c r="BL11" s="12"/>
+      <c r="BM11" s="12"/>
+      <c r="BN11" s="12"/>
+      <c r="BO11" s="12"/>
+      <c r="BP11" s="12"/>
+      <c r="BQ11" s="16"/>
+      <c r="BR11" s="20"/>
+      <c r="BS11" s="15"/>
+      <c r="BT11" s="15"/>
+      <c r="BU11" s="15"/>
+      <c r="BV11" s="15"/>
+      <c r="BW11" s="15"/>
+      <c r="BX11" s="15"/>
+      <c r="BY11" s="15"/>
+      <c r="BZ11" s="15"/>
+      <c r="CA11" s="15"/>
+      <c r="CB11" s="15"/>
+      <c r="CC11" s="15"/>
+      <c r="CD11" s="15"/>
+      <c r="CE11" s="15"/>
+      <c r="CF11" s="15"/>
+      <c r="CG11" s="15"/>
+      <c r="CH11" s="15"/>
+      <c r="CI11" s="15"/>
+      <c r="CJ11" s="15"/>
+      <c r="CK11" s="15"/>
+      <c r="CL11" s="15"/>
+      <c r="CM11" s="15"/>
+      <c r="CN11" s="27"/>
+      <c r="CO11" s="15"/>
+      <c r="CP11" s="9"/>
+      <c r="CQ11" s="29"/>
+      <c r="CR11" s="15"/>
+      <c r="CS11" s="9"/>
+      <c r="CT11" s="9"/>
+      <c r="CU11" s="9"/>
+      <c r="CV11" s="29"/>
+      <c r="CW11" s="15"/>
+      <c r="CX11" s="9"/>
+      <c r="CY11" s="9"/>
+      <c r="CZ11" s="9"/>
+      <c r="DA11" s="9"/>
+      <c r="DB11" s="9"/>
+      <c r="DC11" s="29"/>
+      <c r="DD11" s="15"/>
+      <c r="DE11" s="29"/>
+      <c r="DF11" s="15"/>
+      <c r="DG11" s="9"/>
+      <c r="DH11" s="9"/>
+      <c r="DI11" s="29"/>
+      <c r="DJ11" s="1">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="DK11" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="2:116" x14ac:dyDescent="0.3">
+      <c r="DJ12" s="6"/>
+    </row>
+    <row r="13" spans="2:116" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="1">
-        <f>COUNTIF(C4:C10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="D12" s="1">
-        <f>COUNTIF(D4:D10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="E12" s="1">
-        <f>COUNTIF(E4:E10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
-        <f>COUNTIF(F4:F10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="G12" s="1">
-        <f>COUNTIF(G4:G10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="H12" s="1">
-        <f>COUNTIF(H4:H10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="I12" s="1">
-        <f>COUNTIF(I4:I10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="J12" s="1">
-        <f>COUNTIF(J4:J10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="K12" s="1">
-        <f>COUNTIF(K4:K10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="L12" s="1">
-        <f>COUNTIF(L4:L10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="M12" s="1">
-        <f>COUNTIF(M4:M10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="N12" s="1">
-        <f>COUNTIF(N4:N10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="O12" s="1">
-        <f>COUNTIF(O4:O10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="P12" s="1">
-        <f>COUNTIF(P4:P10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="Q12" s="1">
-        <f>COUNTIF(Q4:Q10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="R12" s="1">
-        <f>COUNTIF(R4:R10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="S12" s="1">
-        <f>COUNTIF(S4:S10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="T12" s="1">
-        <f>COUNTIF(T4:T10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="U12" s="1">
-        <f>COUNTIF(U4:U10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="V12" s="1">
-        <f>COUNTIF(V4:V10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="W12" s="1">
-        <f>COUNTIF(W4:W10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="X12" s="1">
-        <f>COUNTIF(X4:X10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="Y12" s="1">
-        <f>COUNTIF(Y4:Y10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="Z12" s="1">
-        <f>COUNTIF(Z4:Z10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AA12" s="1">
-        <f>COUNTIF(AA4:AA10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AB12" s="1">
-        <f>COUNTIF(AB4:AB10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AC12" s="1">
-        <f>COUNTIF(AC4:AC10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AD12" s="1">
-        <f>COUNTIF(AD4:AD10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AE12" s="1">
-        <f>COUNTIF(AE4:AE10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AF12" s="1">
-        <f>COUNTIF(AF4:AF10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AG12" s="1">
-        <f>COUNTIF(AG4:AG10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AH12" s="1">
-        <f>COUNTIF(AH4:AH10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AI12" s="1">
-        <f>COUNTIF(AI4:AI10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AJ12" s="1">
-        <f>COUNTIF(AJ4:AJ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AK12" s="1">
-        <f>COUNTIF(AK4:AK10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AL12" s="1">
-        <f>COUNTIF(AL4:AL10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AM12" s="1">
-        <f>COUNTIF(AM4:AM10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AN12" s="1">
-        <f>COUNTIF(AN4:AN10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AO12" s="1">
-        <f>COUNTIF(AO4:AO10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AP12" s="1">
-        <f>COUNTIF(AP4:AP10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AQ12" s="1">
-        <f>COUNTIF(AQ4:AQ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AR12" s="1">
-        <f>COUNTIF(AR4:AR10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AS12" s="1">
-        <f>COUNTIF(AS4:AS10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AT12" s="1">
-        <f>COUNTIF(AT4:AT10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AU12" s="1">
-        <f>COUNTIF(AU4:AU10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AV12" s="1">
-        <f>COUNTIF(AV4:AV10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AW12" s="1">
-        <f>COUNTIF(AW4:AW10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AX12" s="1">
-        <f>COUNTIF(AX4:AX10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AY12" s="1">
-        <f>COUNTIF(AY4:AY10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="AZ12" s="1">
-        <f>COUNTIF(AZ4:AZ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BA12" s="1">
-        <f>COUNTIF(BA4:BA10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BB12" s="1">
-        <f>COUNTIF(BB4:BB10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BC12" s="1">
-        <f>COUNTIF(BC4:BC10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BD12" s="1">
-        <f>COUNTIF(BD4:BD10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BE12" s="1">
-        <f>COUNTIF(BE4:BE10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BF12" s="1">
-        <f>COUNTIF(BF4:BF10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BG12" s="1">
-        <f>COUNTIF(BG4:BG10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BH12" s="1">
-        <f>COUNTIF(BH4:BH10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BI12" s="1">
-        <f>COUNTIF(BI4:BI10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BJ12" s="1">
-        <f>COUNTIF(BJ4:BJ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BK12" s="1">
-        <f>COUNTIF(BK4:BK10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BL12" s="1">
-        <f>COUNTIF(BL4:BL10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BM12" s="1">
-        <f>COUNTIF(BM4:BM10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BN12" s="1">
-        <f>COUNTIF(BN4:BN10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BO12" s="1">
-        <f>COUNTIF(BO4:BO10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BP12" s="1">
-        <f>COUNTIF(BP4:BP10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BQ12" s="1">
-        <f>COUNTIF(BQ4:BQ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BR12" s="1">
-        <f>COUNTIF(BR4:BR10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BS12" s="1">
-        <f>COUNTIF(BS4:BS10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BT12" s="1">
-        <f>COUNTIF(BT4:BT10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BU12" s="1">
-        <f>COUNTIF(BU4:BU10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BV12" s="1">
-        <f>COUNTIF(BV4:BV10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BW12" s="1">
-        <f>COUNTIF(BW4:BW10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BX12" s="1">
-        <f>COUNTIF(BX4:BX10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BY12" s="1">
-        <f>COUNTIF(BY4:BY10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="BZ12" s="1">
-        <f>COUNTIF(BZ4:BZ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CA12" s="1">
-        <f>COUNTIF(CA4:CA10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CB12" s="1">
-        <f>COUNTIF(CB4:CB10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CC12" s="1">
-        <f>COUNTIF(CC4:CC10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CD12" s="1">
-        <f>COUNTIF(CD4:CD10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CE12" s="1">
-        <f>COUNTIF(CE4:CE10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CF12" s="1">
-        <f>COUNTIF(CF4:CF10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CG12" s="1">
-        <f>COUNTIF(CG4:CG10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CH12" s="1">
-        <f>COUNTIF(CH4:CH10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CI12" s="1">
-        <f>COUNTIF(CI4:CI10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CJ12" s="1">
-        <f>COUNTIF(CJ4:CJ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CK12" s="1">
-        <f>COUNTIF(CK4:CK10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CL12" s="1">
-        <f>COUNTIF(CL4:CL10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CM12" s="1">
-        <f>COUNTIF(CM4:CM10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CN12" s="1">
-        <f>COUNTIF(CN4:CN10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CO12" s="1">
-        <f>COUNTIF(CO4:CO10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CP12" s="1">
-        <f>COUNTIF(CP4:CP10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CQ12" s="1">
-        <f>COUNTIF(CQ4:CQ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CR12" s="1">
-        <f>COUNTIF(CR4:CR10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CS12" s="1">
-        <f>COUNTIF(CS4:CS10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CT12" s="1">
-        <f>COUNTIF(CT4:CT10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CU12" s="1">
-        <f>COUNTIF(CU4:CU10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CV12" s="1">
-        <f>COUNTIF(CV4:CV10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CW12" s="1">
-        <f>COUNTIF(CW4:CW10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CX12" s="1">
-        <f>COUNTIF(CX4:CX10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CY12" s="1">
-        <f>COUNTIF(CY4:CY10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="CZ12" s="1">
-        <f>COUNTIF(CZ4:CZ10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DA12" s="1">
-        <f>COUNTIF(DA4:DA10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DB12" s="1">
-        <f>COUNTIF(DB4:DB10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DC12" s="1">
-        <f>COUNTIF(DC4:DC10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DD12" s="1">
-        <f>COUNTIF(DD4:DD10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DE12" s="1">
-        <f>COUNTIF(DE4:DE10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DF12" s="1">
-        <f>COUNTIF(DF4:DF10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DG12" s="1">
-        <f>COUNTIF(DG4:DG10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DH12" s="1">
-        <f>COUNTIF(DH4:DH10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DI12" s="1">
-        <f>COUNTIF(DI4:DI10,"")</f>
-        <v>7</v>
-      </c>
-      <c r="DJ12" s="6">
-        <f>SUM(C12:DI12)</f>
-        <v>777</v>
-      </c>
-      <c r="DK12" s="2"/>
-    </row>
-    <row r="13" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="C13" s="1">
-        <f>COUNTIF(C4:C10,"x")</f>
-        <v>0</v>
+        <f t="shared" ref="C13:AH13" si="2">COUNTIF(C4:C11,"")</f>
+        <v>8</v>
       </c>
       <c r="D13" s="1">
-        <f>COUNTIF(D4:D10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="E13" s="1">
-        <f>COUNTIF(E4:E10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="F13" s="1">
-        <f>COUNTIF(F4:F10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="G13" s="1">
-        <f>COUNTIF(G4:G10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="H13" s="1">
-        <f>COUNTIF(H4:H10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="I13" s="1">
-        <f>COUNTIF(I4:I10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="J13" s="1">
-        <f>COUNTIF(J4:J10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="K13" s="1">
-        <f>COUNTIF(K4:K10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="L13" s="1">
-        <f>COUNTIF(L4:L10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="M13" s="1">
-        <f>COUNTIF(M4:M10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="N13" s="1">
-        <f>COUNTIF(N4:N10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="O13" s="1">
-        <f>COUNTIF(O4:O10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="P13" s="1">
-        <f>COUNTIF(P4:P10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="Q13" s="1">
-        <f>COUNTIF(Q4:Q10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="R13" s="1">
-        <f>COUNTIF(R4:R10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="S13" s="1">
-        <f>COUNTIF(S4:S10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="T13" s="1">
-        <f>COUNTIF(T4:T10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="U13" s="1">
-        <f>COUNTIF(U4:U10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="V13" s="1">
-        <f>COUNTIF(V4:V10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="W13" s="1">
-        <f>COUNTIF(W4:W10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="X13" s="1">
-        <f>COUNTIF(X4:X10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="Y13" s="1">
-        <f>COUNTIF(Y4:Y10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="Z13" s="1">
-        <f>COUNTIF(Z4:Z10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AA13" s="1">
-        <f>COUNTIF(AA4:AA10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AB13" s="1">
-        <f>COUNTIF(AB4:AB10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AC13" s="1">
-        <f>COUNTIF(AC4:AC10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AD13" s="1">
-        <f>COUNTIF(AD4:AD10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AE13" s="1">
-        <f>COUNTIF(AE4:AE10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AF13" s="1">
-        <f>COUNTIF(AF4:AF10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AG13" s="1">
-        <f>COUNTIF(AG4:AG10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AH13" s="1">
-        <f>COUNTIF(AH4:AH10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="AI13" s="1">
-        <f>COUNTIF(AI4:AI10,"x")</f>
-        <v>0</v>
+        <f t="shared" ref="AI13:BN13" si="3">COUNTIF(AI4:AI11,"")</f>
+        <v>8</v>
       </c>
       <c r="AJ13" s="1">
-        <f>COUNTIF(AJ4:AJ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AK13" s="1">
-        <f>COUNTIF(AK4:AK10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AL13" s="1">
-        <f>COUNTIF(AL4:AL10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AM13" s="1">
-        <f>COUNTIF(AM4:AM10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AN13" s="1">
-        <f>COUNTIF(AN4:AN10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AO13" s="1">
-        <f>COUNTIF(AO4:AO10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AP13" s="1">
-        <f>COUNTIF(AP4:AP10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AQ13" s="1">
-        <f>COUNTIF(AQ4:AQ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AR13" s="1">
-        <f>COUNTIF(AR4:AR10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AS13" s="1">
-        <f>COUNTIF(AS4:AS10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AT13" s="1">
-        <f>COUNTIF(AT4:AT10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AU13" s="1">
-        <f>COUNTIF(AU4:AU10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AV13" s="1">
-        <f>COUNTIF(AV4:AV10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AW13" s="1">
-        <f>COUNTIF(AW4:AW10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AX13" s="1">
-        <f>COUNTIF(AX4:AX10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AY13" s="1">
-        <f>COUNTIF(AY4:AY10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AZ13" s="1">
-        <f>COUNTIF(AZ4:AZ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BA13" s="1">
-        <f>COUNTIF(BA4:BA10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BB13" s="1">
-        <f>COUNTIF(BB4:BB10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BC13" s="1">
-        <f>COUNTIF(BC4:BC10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BD13" s="1">
-        <f>COUNTIF(BD4:BD10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BE13" s="1">
-        <f>COUNTIF(BE4:BE10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BF13" s="1">
-        <f>COUNTIF(BF4:BF10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BG13" s="1">
-        <f>COUNTIF(BG4:BG10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BH13" s="1">
-        <f>COUNTIF(BH4:BH10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BI13" s="1">
-        <f>COUNTIF(BI4:BI10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BJ13" s="1">
-        <f>COUNTIF(BJ4:BJ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BK13" s="1">
-        <f>COUNTIF(BK4:BK10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BL13" s="1">
-        <f>COUNTIF(BL4:BL10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BM13" s="1">
-        <f>COUNTIF(BM4:BM10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BN13" s="1">
-        <f>COUNTIF(BN4:BN10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="BO13" s="1">
-        <f>COUNTIF(BO4:BO10,"x")</f>
-        <v>0</v>
+        <f t="shared" ref="BO13:CT13" si="4">COUNTIF(BO4:BO11,"")</f>
+        <v>8</v>
       </c>
       <c r="BP13" s="1">
-        <f>COUNTIF(BP4:BP10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BQ13" s="1">
-        <f>COUNTIF(BQ4:BQ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BR13" s="1">
-        <f>COUNTIF(BR4:BR10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BS13" s="1">
-        <f>COUNTIF(BS4:BS10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BT13" s="1">
-        <f>COUNTIF(BT4:BT10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BU13" s="1">
-        <f>COUNTIF(BU4:BU10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BV13" s="1">
-        <f>COUNTIF(BV4:BV10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BW13" s="1">
-        <f>COUNTIF(BW4:BW10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BX13" s="1">
-        <f>COUNTIF(BX4:BX10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BY13" s="1">
-        <f>COUNTIF(BY4:BY10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="BZ13" s="1">
-        <f>COUNTIF(BZ4:BZ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CA13" s="1">
-        <f>COUNTIF(CA4:CA10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CB13" s="1">
-        <f>COUNTIF(CB4:CB10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CC13" s="1">
-        <f>COUNTIF(CC4:CC10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CD13" s="1">
-        <f>COUNTIF(CD4:CD10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CE13" s="1">
-        <f>COUNTIF(CE4:CE10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CF13" s="1">
-        <f>COUNTIF(CF4:CF10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CG13" s="1">
-        <f>COUNTIF(CG4:CG10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CH13" s="1">
-        <f>COUNTIF(CH4:CH10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CI13" s="1">
-        <f>COUNTIF(CI4:CI10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CJ13" s="1">
-        <f>COUNTIF(CJ4:CJ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CK13" s="1">
-        <f>COUNTIF(CK4:CK10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CL13" s="1">
-        <f>COUNTIF(CL4:CL10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CM13" s="1">
-        <f>COUNTIF(CM4:CM10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CN13" s="1">
-        <f>COUNTIF(CN4:CN10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CO13" s="1">
-        <f>COUNTIF(CO4:CO10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CP13" s="1">
-        <f>COUNTIF(CP4:CP10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CQ13" s="1">
-        <f>COUNTIF(CQ4:CQ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CR13" s="1">
-        <f>COUNTIF(CR4:CR10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CS13" s="1">
-        <f>COUNTIF(CS4:CS10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CT13" s="1">
-        <f>COUNTIF(CT4:CT10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="CU13" s="1">
-        <f>COUNTIF(CU4:CU10,"x")</f>
-        <v>0</v>
+        <f t="shared" ref="CU13:DI13" si="5">COUNTIF(CU4:CU11,"")</f>
+        <v>8</v>
       </c>
       <c r="CV13" s="1">
-        <f>COUNTIF(CV4:CV10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="CW13" s="1">
-        <f>COUNTIF(CW4:CW10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="CX13" s="1">
-        <f>COUNTIF(CX4:CX10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="CY13" s="1">
-        <f>COUNTIF(CY4:CY10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="CZ13" s="1">
-        <f>COUNTIF(CZ4:CZ10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DA13" s="1">
-        <f>COUNTIF(DA4:DA10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DB13" s="1">
-        <f>COUNTIF(DB4:DB10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DC13" s="1">
-        <f>COUNTIF(DC4:DC10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DD13" s="1">
-        <f>COUNTIF(DD4:DD10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DE13" s="1">
-        <f>COUNTIF(DE4:DE10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DF13" s="1">
-        <f>COUNTIF(DF4:DF10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DG13" s="1">
-        <f>COUNTIF(DG4:DG10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DH13" s="1">
-        <f>COUNTIF(DH4:DH10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DI13" s="1">
-        <f>COUNTIF(DI4:DI10,"x")</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="DJ13" s="6">
-        <f t="shared" ref="DJ13:DJ15" si="2">SUM(C13:DI13)</f>
-        <v>0</v>
+        <f>SUM(C13:DI13)</f>
+        <v>888</v>
       </c>
       <c r="DK13" s="2"/>
     </row>
-    <row r="14" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:116" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:AH14" si="6">COUNTIF(C4:C11,"x")</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AG14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="1">
+        <f t="shared" ref="AI14:BN14" si="7">COUNTIF(AI4:AI11,"x")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AK14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AL14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AM14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AN14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AO14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AP14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AR14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AS14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AT14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AU14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AV14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AW14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AX14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AY14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AZ14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BA14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BB14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BC14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BD14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BE14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BF14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BG14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BH14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BI14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BJ14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BK14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BL14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BM14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BN14" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BO14" s="1">
+        <f t="shared" ref="BO14:CT14" si="8">COUNTIF(BO4:BO11,"x")</f>
+        <v>0</v>
+      </c>
+      <c r="BP14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BQ14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BR14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BS14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BT14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BU14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BV14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BW14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BX14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BY14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BZ14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CA14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CB14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CC14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CD14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CE14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CF14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CG14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CH14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CI14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CJ14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CK14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CL14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CM14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CN14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CO14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CP14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CQ14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CR14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CS14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CT14" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CU14" s="1">
+        <f t="shared" ref="CU14:DI14" si="9">COUNTIF(CU4:CU11,"x")</f>
+        <v>0</v>
+      </c>
+      <c r="CV14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="CW14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="CX14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="CY14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="CZ14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DA14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DB14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DC14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DD14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DE14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DF14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DG14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DH14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DI14" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DJ14" s="6">
+        <f t="shared" ref="DJ14:DJ16" si="10">SUM(C14:DI14)</f>
+        <v>0</v>
+      </c>
+      <c r="DK14" s="2"/>
+    </row>
+    <row r="15" spans="2:116" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="1">
-        <f>COUNTIF(C4:C10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <f>COUNTIF(D4:D10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <f>COUNTIF(E4:E10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <f>COUNTIF(F4:F10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <f>COUNTIF(G4:G10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <f>COUNTIF(H4:H10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <f>COUNTIF(I4:I10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <f>COUNTIF(J4:J10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
-        <f>COUNTIF(K4:K10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="1">
-        <f>COUNTIF(L4:L10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="1">
-        <f>COUNTIF(M4:M10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <f>COUNTIF(N4:N10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="1">
-        <f>COUNTIF(O4:O10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <f>COUNTIF(P4:P10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <f>COUNTIF(Q4:Q10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="R14" s="1">
-        <f>COUNTIF(R4:R10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="1">
-        <f>COUNTIF(S4:S10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="T14" s="1">
-        <f>COUNTIF(T4:T10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="U14" s="1">
-        <f>COUNTIF(U4:U10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="V14" s="1">
-        <f>COUNTIF(V4:V10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="W14" s="1">
-        <f>COUNTIF(W4:W10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="X14" s="1">
-        <f>COUNTIF(X4:X10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="Y14" s="1">
-        <f>COUNTIF(Y4:Y10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="1">
-        <f>COUNTIF(Z4:Z10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AA14" s="1">
-        <f>COUNTIF(AA4:AA10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="1">
-        <f>COUNTIF(AB4:AB10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AC14" s="1">
-        <f>COUNTIF(AC4:AC10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AD14" s="1">
-        <f>COUNTIF(AD4:AD10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AE14" s="1">
-        <f>COUNTIF(AE4:AE10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AF14" s="1">
-        <f>COUNTIF(AF4:AF10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AG14" s="1">
-        <f>COUNTIF(AG4:AG10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AH14" s="1">
-        <f>COUNTIF(AH4:AH10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AI14" s="1">
-        <f>COUNTIF(AI4:AI10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="1">
-        <f>COUNTIF(AJ4:AJ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AK14" s="1">
-        <f>COUNTIF(AK4:AK10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AL14" s="1">
-        <f>COUNTIF(AL4:AL10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AM14" s="1">
-        <f>COUNTIF(AM4:AM10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AN14" s="1">
-        <f>COUNTIF(AN4:AN10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AO14" s="1">
-        <f>COUNTIF(AO4:AO10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AP14" s="1">
-        <f>COUNTIF(AP4:AP10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="1">
-        <f>COUNTIF(AQ4:AQ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AR14" s="1">
-        <f>COUNTIF(AR4:AR10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AS14" s="1">
-        <f>COUNTIF(AS4:AS10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AT14" s="1">
-        <f>COUNTIF(AT4:AT10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AU14" s="1">
-        <f>COUNTIF(AU4:AU10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AV14" s="1">
-        <f>COUNTIF(AV4:AV10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AW14" s="1">
-        <f>COUNTIF(AW4:AW10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AX14" s="1">
-        <f>COUNTIF(AX4:AX10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AY14" s="1">
-        <f>COUNTIF(AY4:AY10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="1">
-        <f>COUNTIF(AZ4:AZ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BA14" s="1">
-        <f>COUNTIF(BA4:BA10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BB14" s="1">
-        <f>COUNTIF(BB4:BB10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BC14" s="1">
-        <f>COUNTIF(BC4:BC10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BD14" s="1">
-        <f>COUNTIF(BD4:BD10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BE14" s="1">
-        <f>COUNTIF(BE4:BE10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BF14" s="1">
-        <f>COUNTIF(BF4:BF10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BG14" s="1">
-        <f>COUNTIF(BG4:BG10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BH14" s="1">
-        <f>COUNTIF(BH4:BH10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BI14" s="1">
-        <f>COUNTIF(BI4:BI10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ14" s="1">
-        <f>COUNTIF(BJ4:BJ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BK14" s="1">
-        <f>COUNTIF(BK4:BK10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BL14" s="1">
-        <f>COUNTIF(BL4:BL10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BM14" s="1">
-        <f>COUNTIF(BM4:BM10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BN14" s="1">
-        <f>COUNTIF(BN4:BN10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BO14" s="1">
-        <f>COUNTIF(BO4:BO10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BP14" s="1">
-        <f>COUNTIF(BP4:BP10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BQ14" s="1">
-        <f>COUNTIF(BQ4:BQ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BR14" s="1">
-        <f>COUNTIF(BR4:BR10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BS14" s="1">
-        <f>COUNTIF(BS4:BS10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BT14" s="1">
-        <f>COUNTIF(BT4:BT10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BU14" s="1">
-        <f>COUNTIF(BU4:BU10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BV14" s="1">
-        <f>COUNTIF(BV4:BV10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BW14" s="1">
-        <f>COUNTIF(BW4:BW10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BX14" s="1">
-        <f>COUNTIF(BX4:BX10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BY14" s="1">
-        <f>COUNTIF(BY4:BY10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="BZ14" s="1">
-        <f>COUNTIF(BZ4:BZ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CA14" s="1">
-        <f>COUNTIF(CA4:CA10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CB14" s="1">
-        <f>COUNTIF(CB4:CB10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CC14" s="1">
-        <f>COUNTIF(CC4:CC10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CD14" s="1">
-        <f>COUNTIF(CD4:CD10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CE14" s="1">
-        <f>COUNTIF(CE4:CE10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CF14" s="1">
-        <f>COUNTIF(CF4:CF10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CG14" s="1">
-        <f>COUNTIF(CG4:CG10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CH14" s="1">
-        <f>COUNTIF(CH4:CH10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CI14" s="1">
-        <f>COUNTIF(CI4:CI10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CJ14" s="1">
-        <f>COUNTIF(CJ4:CJ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CK14" s="1">
-        <f>COUNTIF(CK4:CK10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CL14" s="1">
-        <f>COUNTIF(CL4:CL10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CM14" s="1">
-        <f>COUNTIF(CM4:CM10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CN14" s="1">
-        <f>COUNTIF(CN4:CN10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CO14" s="1">
-        <f>COUNTIF(CO4:CO10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CP14" s="1">
-        <f>COUNTIF(CP4:CP10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CQ14" s="1">
-        <f>COUNTIF(CQ4:CQ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CR14" s="1">
-        <f>COUNTIF(CR4:CR10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CS14" s="1">
-        <f>COUNTIF(CS4:CS10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CT14" s="1">
-        <f>COUNTIF(CT4:CT10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CU14" s="1">
-        <f>COUNTIF(CU4:CU10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CV14" s="1">
-        <f>COUNTIF(CV4:CV10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CW14" s="1">
-        <f>COUNTIF(CW4:CW10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CX14" s="1">
-        <f>COUNTIF(CX4:CX10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CY14" s="1">
-        <f>COUNTIF(CY4:CY10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="CZ14" s="1">
-        <f>COUNTIF(CZ4:CZ10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DA14" s="1">
-        <f>COUNTIF(DA4:DA10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DB14" s="1">
-        <f>COUNTIF(DB4:DB10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DC14" s="1">
-        <f>COUNTIF(DC4:DC10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DD14" s="1">
-        <f>COUNTIF(DD4:DD10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DE14" s="1">
-        <f>COUNTIF(DE4:DE10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DF14" s="1">
-        <f>COUNTIF(DF4:DF10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DG14" s="1">
-        <f>COUNTIF(DG4:DG10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DH14" s="1">
-        <f>COUNTIF(DH4:DH10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DI14" s="1">
-        <f>COUNTIF(DI4:DI10,"p")</f>
-        <v>0</v>
-      </c>
-      <c r="DJ14" s="6">
-        <f t="shared" si="2"/>
+      <c r="C15" s="1">
+        <f t="shared" ref="C15:AH15" si="11">COUNTIF(C4:C11,"p")</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AF15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AG15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AI15" s="1">
+        <f t="shared" ref="AI15:BN15" si="12">COUNTIF(AI4:AI11,"p")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AK15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AL15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AM15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AN15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AO15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AP15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AR15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AS15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AT15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AV15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AW15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AX15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AY15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AZ15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BA15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BB15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BC15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BD15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BE15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BF15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BG15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BH15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BI15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BJ15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BK15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BL15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BM15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BN15" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BO15" s="1">
+        <f t="shared" ref="BO15:CT15" si="13">COUNTIF(BO4:BO11,"p")</f>
+        <v>0</v>
+      </c>
+      <c r="BP15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BQ15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BR15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BS15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BT15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BU15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BV15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BW15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BX15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BY15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BZ15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CA15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CB15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CC15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CD15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CE15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CF15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CG15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CH15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CI15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CJ15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CK15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CL15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CM15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CN15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CO15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CP15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CQ15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CR15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CS15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CT15" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="CU15" s="1">
+        <f t="shared" ref="CU15:DI15" si="14">COUNTIF(CU4:CU11,"p")</f>
+        <v>0</v>
+      </c>
+      <c r="CV15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="CW15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="CX15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="CY15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="CZ15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DA15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DB15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DC15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DD15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DE15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DF15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DG15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DH15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DI15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="DJ15" s="6">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:116" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+    <row r="16" spans="2:116" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="1">
-        <f>COUNTIF(C4:C10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <f>COUNTIF(D4:D10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <f>COUNTIF(E4:E10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <f>COUNTIF(F4:F10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <f>COUNTIF(G4:G10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <f>COUNTIF(H4:H10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <f>COUNTIF(I4:I10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <f>COUNTIF(J4:J10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <f>COUNTIF(K4:K10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
-        <f>COUNTIF(L4:L10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="1">
-        <f>COUNTIF(M4:M10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <f>COUNTIF(N4:N10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <f>COUNTIF(O4:O10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <f>COUNTIF(P4:P10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <f>COUNTIF(Q4:Q10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="1">
-        <f>COUNTIF(R4:R10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="1">
-        <f>COUNTIF(S4:S10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="1">
-        <f>COUNTIF(T4:T10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="U15" s="1">
-        <f>COUNTIF(U4:U10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="V15" s="1">
-        <f>COUNTIF(V4:V10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="W15" s="1">
-        <f>COUNTIF(W4:W10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="X15" s="1">
-        <f>COUNTIF(X4:X10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="Y15" s="1">
-        <f>COUNTIF(Y4:Y10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="1">
-        <f>COUNTIF(Z4:Z10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="1">
-        <f>COUNTIF(AA4:AA10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AB15" s="1">
-        <f>COUNTIF(AB4:AB10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AC15" s="1">
-        <f>COUNTIF(AC4:AC10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AD15" s="1">
-        <f>COUNTIF(AD4:AD10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AE15" s="1">
-        <f>COUNTIF(AE4:AE10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AF15" s="1">
-        <f>COUNTIF(AF4:AF10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AG15" s="1">
-        <f>COUNTIF(AG4:AG10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AH15" s="1">
-        <f>COUNTIF(AH4:AH10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AI15" s="1">
-        <f>COUNTIF(AI4:AI10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="1">
-        <f>COUNTIF(AJ4:AJ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AK15" s="1">
-        <f>COUNTIF(AK4:AK10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AL15" s="1">
-        <f>COUNTIF(AL4:AL10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AM15" s="1">
-        <f>COUNTIF(AM4:AM10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AN15" s="1">
-        <f>COUNTIF(AN4:AN10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AO15" s="1">
-        <f>COUNTIF(AO4:AO10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AP15" s="1">
-        <f>COUNTIF(AP4:AP10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="1">
-        <f>COUNTIF(AQ4:AQ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AR15" s="1">
-        <f>COUNTIF(AR4:AR10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AS15" s="1">
-        <f>COUNTIF(AS4:AS10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AT15" s="1">
-        <f>COUNTIF(AT4:AT10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AU15" s="1">
-        <f>COUNTIF(AU4:AU10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AV15" s="1">
-        <f>COUNTIF(AV4:AV10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AW15" s="1">
-        <f>COUNTIF(AW4:AW10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AX15" s="1">
-        <f>COUNTIF(AX4:AX10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AY15" s="1">
-        <f>COUNTIF(AY4:AY10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AZ15" s="1">
-        <f>COUNTIF(AZ4:AZ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BA15" s="1">
-        <f>COUNTIF(BA4:BA10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BB15" s="1">
-        <f>COUNTIF(BB4:BB10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BC15" s="1">
-        <f>COUNTIF(BC4:BC10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BD15" s="1">
-        <f>COUNTIF(BD4:BD10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BE15" s="1">
-        <f>COUNTIF(BE4:BE10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BF15" s="1">
-        <f>COUNTIF(BF4:BF10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BG15" s="1">
-        <f>COUNTIF(BG4:BG10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BH15" s="1">
-        <f>COUNTIF(BH4:BH10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BI15" s="1">
-        <f>COUNTIF(BI4:BI10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BJ15" s="1">
-        <f>COUNTIF(BJ4:BJ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BK15" s="1">
-        <f>COUNTIF(BK4:BK10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BL15" s="1">
-        <f>COUNTIF(BL4:BL10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BM15" s="1">
-        <f>COUNTIF(BM4:BM10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BN15" s="1">
-        <f>COUNTIF(BN4:BN10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BO15" s="1">
-        <f>COUNTIF(BO4:BO10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BP15" s="1">
-        <f>COUNTIF(BP4:BP10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BQ15" s="1">
-        <f>COUNTIF(BQ4:BQ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BR15" s="1">
-        <f>COUNTIF(BR4:BR10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BS15" s="1">
-        <f>COUNTIF(BS4:BS10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BT15" s="1">
-        <f>COUNTIF(BT4:BT10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BU15" s="1">
-        <f>COUNTIF(BU4:BU10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BV15" s="1">
-        <f>COUNTIF(BV4:BV10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BW15" s="1">
-        <f>COUNTIF(BW4:BW10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BX15" s="1">
-        <f>COUNTIF(BX4:BX10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BY15" s="1">
-        <f>COUNTIF(BY4:BY10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="BZ15" s="1">
-        <f>COUNTIF(BZ4:BZ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CA15" s="1">
-        <f>COUNTIF(CA4:CA10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CB15" s="1">
-        <f>COUNTIF(CB4:CB10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CC15" s="1">
-        <f>COUNTIF(CC4:CC10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CD15" s="1">
-        <f>COUNTIF(CD4:CD10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CE15" s="1">
-        <f>COUNTIF(CE4:CE10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CF15" s="1">
-        <f>COUNTIF(CF4:CF10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CG15" s="1">
-        <f>COUNTIF(CG4:CG10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CH15" s="1">
-        <f>COUNTIF(CH4:CH10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CI15" s="1">
-        <f>COUNTIF(CI4:CI10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CJ15" s="1">
-        <f>COUNTIF(CJ4:CJ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CK15" s="1">
-        <f>COUNTIF(CK4:CK10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CL15" s="1">
-        <f>COUNTIF(CL4:CL10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CM15" s="1">
-        <f>COUNTIF(CM4:CM10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CN15" s="1">
-        <f>COUNTIF(CN4:CN10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CO15" s="1">
-        <f>COUNTIF(CO4:CO10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CP15" s="1">
-        <f>COUNTIF(CP4:CP10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CQ15" s="1">
-        <f>COUNTIF(CQ4:CQ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CR15" s="1">
-        <f>COUNTIF(CR4:CR10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CS15" s="1">
-        <f>COUNTIF(CS4:CS10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CT15" s="1">
-        <f>COUNTIF(CT4:CT10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CU15" s="1">
-        <f>COUNTIF(CU4:CU10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CV15" s="1">
-        <f>COUNTIF(CV4:CV10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CW15" s="1">
-        <f>COUNTIF(CW4:CW10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CX15" s="1">
-        <f>COUNTIF(CX4:CX10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CY15" s="1">
-        <f>COUNTIF(CY4:CY10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="CZ15" s="1">
-        <f>COUNTIF(CZ4:CZ10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DA15" s="1">
-        <f>COUNTIF(DA4:DA10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DB15" s="1">
-        <f>COUNTIF(DB4:DB10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DC15" s="1">
-        <f>COUNTIF(DC4:DC10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DD15" s="1">
-        <f>COUNTIF(DD4:DD10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DE15" s="1">
-        <f>COUNTIF(DE4:DE10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DF15" s="1">
-        <f>COUNTIF(DF4:DF10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DG15" s="1">
-        <f>COUNTIF(DG4:DG10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DH15" s="1">
-        <f>COUNTIF(DH4:DH10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DI15" s="1">
-        <f>COUNTIF(DI4:DI10,"-")</f>
-        <v>0</v>
-      </c>
-      <c r="DJ15" s="6">
-        <f t="shared" si="2"/>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:AH16" si="15">COUNTIF(C4:C11,"-")</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH16" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="1">
+        <f t="shared" ref="AI16:BN16" si="16">COUNTIF(AI4:AI11,"-")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AK16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AL16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AM16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AO16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AR16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AS16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AT16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AU16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AV16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AW16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AX16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AY16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BA16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BB16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BC16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BD16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BE16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BF16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BG16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BH16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BI16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BK16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BL16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BM16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BN16" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="BO16" s="1">
+        <f t="shared" ref="BO16:CT16" si="17">COUNTIF(BO4:BO11,"-")</f>
+        <v>0</v>
+      </c>
+      <c r="BP16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BQ16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BR16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BS16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BT16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BU16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BV16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BW16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BX16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BY16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BZ16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CA16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CB16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CC16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CD16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CE16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CF16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CG16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CH16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CI16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CJ16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CK16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CL16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CM16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CN16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CO16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CP16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CQ16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CR16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CS16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CT16" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="CU16" s="1">
+        <f t="shared" ref="CU16:DI16" si="18">COUNTIF(CU4:CU11,"-")</f>
+        <v>0</v>
+      </c>
+      <c r="CV16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="CW16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="CX16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="CY16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="CZ16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DA16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DB16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DC16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DD16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DE16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DF16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DG16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DH16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DI16" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="DJ16" s="6">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="CO1:DI1"/>
+    <mergeCell ref="CO2:CQ2"/>
+    <mergeCell ref="CR2:CV2"/>
+    <mergeCell ref="CW2:DC2"/>
+    <mergeCell ref="DD2:DE2"/>
+    <mergeCell ref="DF2:DI2"/>
     <mergeCell ref="BI2:BQ2"/>
     <mergeCell ref="BS2:CD2"/>
     <mergeCell ref="B1:B3"/>
@@ -4697,19 +4817,13 @@
     <mergeCell ref="AG2:AP2"/>
     <mergeCell ref="AQ2:AZ2"/>
     <mergeCell ref="BA2:BF2"/>
-    <mergeCell ref="CO1:DI1"/>
-    <mergeCell ref="CO2:CQ2"/>
-    <mergeCell ref="CR2:CV2"/>
-    <mergeCell ref="CW2:DC2"/>
-    <mergeCell ref="DD2:DE2"/>
-    <mergeCell ref="DF2:DI2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:D10">
+  <conditionalFormatting sqref="C4:D11">
     <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(C4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:DI10">
+  <conditionalFormatting sqref="C4:DI11">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
@@ -4717,7 +4831,7 @@
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:DI15">
+  <conditionalFormatting sqref="C13:DI16">
     <cfRule type="colorScale" priority="226">
       <colorScale>
         <cfvo type="min"/>
@@ -4729,12 +4843,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:DI10">
+  <conditionalFormatting sqref="E4:DI11">
     <cfRule type="containsBlanks" dxfId="0" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DK4:DK10">
+  <conditionalFormatting sqref="DK4:DK11">
     <cfRule type="colorScale" priority="227">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>